<commit_message>
Fix a couple of tests with grouping
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/ExcelDataSourcePanelTest/TestGroupResultHorizontal.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/ExcelDataSourcePanelTest/TestGroupResultHorizontal.xlsx
@@ -405,16 +405,10 @@
       <x:c r="B2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
       <x:c r="D2" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
@@ -434,16 +428,7 @@
       <x:c r="C3" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s"/>
-      <x:c r="F3" s="0" t="s"/>
-      <x:c r="G3" s="0" t="s"/>
       <x:c r="H3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
@@ -451,21 +436,13 @@
       <x:c r="B4" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="b">
-        <x:v>1</x:v>
-      </x:c>
       <x:c r="D4" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="s"/>
-      <x:c r="F4" s="0" t="s"/>
       <x:c r="G4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H4" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I4" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -473,12 +450,6 @@
       <x:c r="B5" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C5" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
       <x:c r="E5" s="0" t="n">
         <x:v>56</x:v>
       </x:c>
@@ -489,9 +460,6 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="H5" s="0" t="n">
-        <x:v>77.7</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="n">
         <x:v>77.7</x:v>
       </x:c>
     </x:row>
@@ -502,37 +470,34 @@
       <x:c r="C6" s="1">
         <x:v>43151</x:v>
       </x:c>
-      <x:c r="D6" s="1">
-        <x:v>43151</x:v>
-      </x:c>
+      <x:c r="D6" s="1" t="s"/>
       <x:c r="E6" s="1">
         <x:v>43149</x:v>
       </x:c>
-      <x:c r="F6" s="0" t="s"/>
-      <x:c r="G6" s="0" t="s"/>
       <x:c r="H6" s="1">
         <x:v>43152</x:v>
       </x:c>
-      <x:c r="I6" s="1">
-        <x:v>43152</x:v>
-      </x:c>
+      <x:c r="I6" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="23">
+  <x:mergeCells count="26">
     <x:mergeCell ref="B3:B3"/>
     <x:mergeCell ref="B6:B6"/>
     <x:mergeCell ref="B2:C2"/>
     <x:mergeCell ref="B4:C4"/>
+    <x:mergeCell ref="B5:C5"/>
     <x:mergeCell ref="D2:D2"/>
     <x:mergeCell ref="C3:D3"/>
     <x:mergeCell ref="D4:D4"/>
-    <x:mergeCell ref="B5:D5"/>
+    <x:mergeCell ref="D5:D5"/>
     <x:mergeCell ref="C6:D6"/>
+    <x:mergeCell ref="E2:E2"/>
     <x:mergeCell ref="E5:E5"/>
     <x:mergeCell ref="E6:E6"/>
+    <x:mergeCell ref="F2:F2"/>
     <x:mergeCell ref="E4:F4"/>
     <x:mergeCell ref="F5:F5"/>
-    <x:mergeCell ref="E2:G2"/>
+    <x:mergeCell ref="G2:G2"/>
     <x:mergeCell ref="E3:G3"/>
     <x:mergeCell ref="G4:G4"/>
     <x:mergeCell ref="G5:G5"/>

</xml_diff>

<commit_message>
Grouping cells takes into account already merged cells + possibility to disable grouping of blank cells
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/ExcelDataSourcePanelTest/TestGroupResultHorizontal.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/ExcelDataSourcePanelTest/TestGroupResultHorizontal.xlsx
@@ -398,13 +398,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:I6"/>
+  <x:dimension ref="A1:J12"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="2" spans="1:9">
+    <x:row r="2" spans="1:10">
       <x:c r="B2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -414,9 +414,6 @@
       <x:c r="E2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
       <x:c r="H2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -424,7 +421,7 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:9">
+    <x:row r="3" spans="1:10">
       <x:c r="B3" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -435,7 +432,7 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:9">
+    <x:row r="4" spans="1:10">
       <x:c r="B4" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
@@ -449,7 +446,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:9">
+    <x:row r="5" spans="1:10">
       <x:c r="B5" s="0">
         <x:v>1</x:v>
       </x:c>
@@ -466,7 +463,7 @@
         <x:v>77.7</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:9">
+    <x:row r="6" spans="1:10">
       <x:c r="B6" s="1">
         <x:v>43149</x:v>
       </x:c>
@@ -484,20 +481,110 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
+    <x:row r="7" spans="1:10">
+      <x:c r="A7" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:10">
+      <x:c r="A8" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:10">
+      <x:c r="A9" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:10">
+      <x:c r="A10" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:10">
+      <x:c r="A11" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I11" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="J11" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:10">
+      <x:c r="A12" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:mergeCells count="12">
+  <x:mergeCells count="21">
     <x:mergeCell ref="B2:C2"/>
-    <x:mergeCell ref="E2:F2"/>
+    <x:mergeCell ref="E2:G2"/>
     <x:mergeCell ref="C3:D3"/>
     <x:mergeCell ref="E3:G3"/>
     <x:mergeCell ref="H3:I3"/>
     <x:mergeCell ref="B4:C4"/>
     <x:mergeCell ref="E4:F4"/>
     <x:mergeCell ref="H4:I4"/>
-    <x:mergeCell ref="B5:C5"/>
+    <x:mergeCell ref="B5:D5"/>
     <x:mergeCell ref="H5:I5"/>
     <x:mergeCell ref="C6:D6"/>
     <x:mergeCell ref="F6:G6"/>
+    <x:mergeCell ref="B7:I7"/>
+    <x:mergeCell ref="C8:I8"/>
+    <x:mergeCell ref="B9:H9"/>
+    <x:mergeCell ref="B10:G10"/>
+    <x:mergeCell ref="H10:I10"/>
+    <x:mergeCell ref="C11:H11"/>
+    <x:mergeCell ref="A12:B12"/>
+    <x:mergeCell ref="C12:G12"/>
+    <x:mergeCell ref="H12:I12"/>
   </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>